<commit_message>
User rep df into sql db
</commit_message>
<xml_diff>
--- a/SRC/DEMO_CODE_drivers.xlsx
+++ b/SRC/DEMO_CODE_drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\OneDrive\Рабочий стол\SANDBOX\DEMO_CODE\SRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8D6DE0-8339-48EA-95B0-1694DFD400BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F89E25-D95A-4BD0-B758-86D55E9630BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>BMW 3 Series С456НУ799, #Е111НС120О33</t>
   </si>
   <si>
-    <t>BMW X3 С234ОР799, #О987УС120У33</t>
-  </si>
-  <si>
     <t>BMW 7 Series У512ОУ777, #У799СС120У33</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>Mercedes-Benz C-Class У798ОН799, #Е797СО120О33</t>
   </si>
   <si>
-    <t>Mercedes-Benz GLE О123ЕР799, #С789ЕС120Е33</t>
-  </si>
-  <si>
     <t>Mercedes-Benz A-Class Р234ОС799, #Е987СС120У33</t>
   </si>
   <si>
@@ -190,12 +184,6 @@
     <t>Chevrolet Traverse О987РЕ797, #Е234КС650Х55</t>
   </si>
   <si>
-    <t>Chevrolet Silverado Е456СР799, #Р678СО120Н22</t>
-  </si>
-  <si>
-    <t>Ford Mustang Р123РХ799, #С361СС920У33</t>
-  </si>
-  <si>
     <t>БЗ-00008</t>
   </si>
   <si>
@@ -295,9 +283,6 @@
     <t>Ford Escape У799СС799, #F359LR120G33</t>
   </si>
   <si>
-    <t>Toyota Prius О777ОР799, #D797QQ120Е33</t>
-  </si>
-  <si>
     <t>BMW 5 Series О789РО799, #L123РР120Е33</t>
   </si>
   <si>
@@ -305,6 +290,21 @@
   </si>
   <si>
     <t>Mercedes-Benz S-Class У512УУ799, #S799SS120Р33</t>
+  </si>
+  <si>
+    <t>BMW X3 #О987УС120У33, С234ОР799</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz GLE #С789ЕС120Е33, ddd00ef, О123ЕР799</t>
+  </si>
+  <si>
+    <t>Toyota Prius #У797АА120С33, О777ОР799, #D797QQ120Е33</t>
+  </si>
+  <si>
+    <t>Ford Mustang D123SS799, #С361СС920У33, Р123РХ799</t>
+  </si>
+  <si>
+    <t>Chevrolet Silverado #Р678СО120Н22, Е456СР799</t>
   </si>
 </sst>
 </file>
@@ -852,8 +852,8 @@
   </sheetPr>
   <dimension ref="B1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="10" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
@@ -972,7 +972,7 @@
     </row>
     <row r="14" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>11</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="15" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>11</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="16" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>11</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="17" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>11</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="18" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>11</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="19" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>11</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="20" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>11</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="23" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B23" s="13" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>11</v>
@@ -1144,7 +1144,7 @@
         <v>4570</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G23" s="11">
         <v>4.8</v>
@@ -1164,7 +1164,7 @@
         <v>5753</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G24" s="11">
         <v>4.5999999999999996</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="25" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>11</v>
@@ -1184,7 +1184,7 @@
         <v>2727</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G25" s="11">
         <v>3.9</v>
@@ -1204,7 +1204,7 @@
         <v>5044</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G26" s="11">
         <v>4.2</v>
@@ -1224,7 +1224,7 @@
         <v>5537</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G27" s="11">
         <v>4.5</v>
@@ -1261,10 +1261,10 @@
         <v>39871.357118055559</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G30" s="11">
         <v>4.8</v>
@@ -1281,10 +1281,10 @@
         <v>39883.383819444447</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G31" s="11">
         <v>4.3</v>
@@ -1304,7 +1304,7 @@
         <v>2135</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G32" s="11">
         <v>4.5</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="33" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>11</v>
@@ -1324,7 +1324,7 @@
         <v>2134</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G33" s="11">
         <v>4.2</v>
@@ -1344,7 +1344,7 @@
         <v>2137</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G34" s="11">
         <v>4.9000000000000004</v>
@@ -1361,10 +1361,10 @@
         <v>41519.650902777779</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G35" s="11">
         <v>3.9</v>
@@ -1384,7 +1384,7 @@
         <v>2136</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G36" s="11">
         <v>4.5999999999999996</v>
@@ -1424,7 +1424,7 @@
         <v>3962</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G39" s="11">
         <v>4.9000000000000004</v>
@@ -1444,7 +1444,7 @@
         <v>4028</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G40" s="11">
         <v>4.3</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="41" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B41" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>11</v>
@@ -1464,7 +1464,7 @@
         <v>3199</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G41" s="11">
         <v>4.2</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="42" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B42" s="8" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>11</v>
@@ -1484,7 +1484,7 @@
         <v>3068</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G42" s="11">
         <v>3.9</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="43" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B43" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>11</v>
@@ -1504,7 +1504,7 @@
         <v>3067</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G43" s="11">
         <v>4.5</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="44" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B44" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>11</v>
@@ -1524,7 +1524,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G44" s="11">
         <v>4.5999999999999996</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="47" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B47" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>11</v>
@@ -1564,7 +1564,7 @@
         <v>4564</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G47" s="11">
         <v>4.9000000000000004</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="48" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B48" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>11</v>
@@ -1581,10 +1581,10 @@
         <v>39758.427395833336</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G48" s="11">
         <v>4.3</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="49" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B49" s="8" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>11</v>
@@ -1601,10 +1601,10 @@
         <v>43161.573599537034</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G49" s="11">
         <v>4.2</v>
@@ -1612,7 +1612,7 @@
     </row>
     <row r="50" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B50" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>11</v>
@@ -1621,10 +1621,10 @@
         <v>43221.400833333333</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G50" s="11">
         <v>3.9</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="51" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="B51" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>11</v>
@@ -1644,7 +1644,7 @@
         <v>4379</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G51" s="11">
         <v>4.5</v>

</xml_diff>

<commit_message>
sql request modules are under reconstruction
</commit_message>
<xml_diff>
--- a/SRC/DEMO_CODE_drivers.xlsx
+++ b/SRC/DEMO_CODE_drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\OneDrive\Рабочий стол\SANDBOX\DEMO_CODE\SRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F89E25-D95A-4BD0-B758-86D55E9630BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A03892-EFF2-479B-8394-A6B71498BC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
@@ -852,18 +852,18 @@
   </sheetPr>
   <dimension ref="B1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="10" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.83203125" defaultRowHeight="11.25" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" customWidth="1"/>
+    <col min="2" max="2" width="59.5" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1187,7 +1187,7 @@
         <v>59</v>
       </c>
       <c r="G25" s="11">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -1367,7 +1367,7 @@
         <v>67</v>
       </c>
       <c r="G35" s="11">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -1627,7 +1627,7 @@
         <v>78</v>
       </c>
       <c r="G50" s="11">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="12" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">

</xml_diff>